<commit_message>
trying to download files for ranges.
</commit_message>
<xml_diff>
--- a/Data/Input/DataInput.xlsx
+++ b/Data/Input/DataInput.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ATM ID</t>
   </si>
@@ -33,13 +33,22 @@
     <t>Type</t>
   </si>
   <si>
-    <t>00000690</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>14/11/2020</t>
+  </si>
+  <si>
     <t>Raya</t>
+  </si>
+  <si>
+    <t>038</t>
   </si>
 </sst>
 </file>
@@ -359,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,11 +381,12 @@
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -390,33 +400,39 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>43932</v>
       </c>
-      <c r="D2" s="1">
-        <v>43932</v>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The happy flow for RAYA and NCR after adding the logic of dividing the date range into days.
</commit_message>
<xml_diff>
--- a/Data/Input/DataInput.xlsx
+++ b/Data/Input/DataInput.xlsx
@@ -42,13 +42,13 @@
     <t>0</t>
   </si>
   <si>
-    <t>14/11/2020</t>
-  </si>
-  <si>
-    <t>Raya</t>
-  </si>
-  <si>
-    <t>038</t>
+    <t>00000690</t>
+  </si>
+  <si>
+    <t>NCR</t>
+  </si>
+  <si>
+    <t>Success</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,16 +409,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
-        <v>43932</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>44085</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44146</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -437,5 +440,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>